<commit_message>
Atualizado por script em 05-01-2024 14:45
</commit_message>
<xml_diff>
--- a/2023/turkey_super-lig_2023-2024.xlsx
+++ b/2023/turkey_super-lig_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V170"/>
+  <dimension ref="A1:V171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15017,71 +15017,71 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Besiktas</t>
+          <t>Ankaragucu</t>
         </is>
       </c>
       <c r="G159" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Alanyaspor</t>
+          <t>Hatayspor</t>
         </is>
       </c>
       <c r="I159" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J159" t="n">
-        <v>1.43</v>
+        <v>1.97</v>
       </c>
       <c r="K159" t="inlineStr">
         <is>
-          <t>14/12/2023 18:12</t>
+          <t>14/12/2023 18:13</t>
         </is>
       </c>
       <c r="L159" t="n">
-        <v>1.64</v>
+        <v>2.27</v>
       </c>
       <c r="M159" t="inlineStr">
         <is>
-          <t>21/12/2023 17:55</t>
+          <t>21/12/2023 17:56</t>
         </is>
       </c>
       <c r="N159" t="n">
-        <v>4.9</v>
+        <v>3.67</v>
       </c>
       <c r="O159" t="inlineStr">
         <is>
-          <t>14/12/2023 18:12</t>
+          <t>14/12/2023 18:13</t>
         </is>
       </c>
       <c r="P159" t="n">
-        <v>4.32</v>
+        <v>3.45</v>
       </c>
       <c r="Q159" t="inlineStr">
         <is>
-          <t>21/12/2023 17:55</t>
+          <t>21/12/2023 17:59</t>
         </is>
       </c>
       <c r="R159" t="n">
-        <v>7</v>
+        <v>3.82</v>
       </c>
       <c r="S159" t="inlineStr">
         <is>
-          <t>14/12/2023 18:12</t>
+          <t>14/12/2023 18:13</t>
         </is>
       </c>
       <c r="T159" t="n">
-        <v>5.26</v>
+        <v>3.36</v>
       </c>
       <c r="U159" t="inlineStr">
         <is>
-          <t>21/12/2023 17:57</t>
+          <t>21/12/2023 17:59</t>
         </is>
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/turkey/super-lig/besiktas-alanyaspor/l41mOf3s/</t>
+          <t>https://www.betexplorer.com/football/turkey/super-lig/ankaragucu-hatayspor/Iw6iNEIm/</t>
         </is>
       </c>
     </row>
@@ -15109,71 +15109,71 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Ankaragucu</t>
+          <t>Besiktas</t>
         </is>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Hatayspor</t>
+          <t>Alanyaspor</t>
         </is>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J160" t="n">
-        <v>1.97</v>
+        <v>1.43</v>
       </c>
       <c r="K160" t="inlineStr">
         <is>
-          <t>14/12/2023 18:13</t>
+          <t>14/12/2023 18:12</t>
         </is>
       </c>
       <c r="L160" t="n">
-        <v>2.27</v>
+        <v>1.64</v>
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>21/12/2023 17:56</t>
+          <t>21/12/2023 17:55</t>
         </is>
       </c>
       <c r="N160" t="n">
-        <v>3.67</v>
+        <v>4.9</v>
       </c>
       <c r="O160" t="inlineStr">
         <is>
-          <t>14/12/2023 18:13</t>
+          <t>14/12/2023 18:12</t>
         </is>
       </c>
       <c r="P160" t="n">
-        <v>3.45</v>
+        <v>4.32</v>
       </c>
       <c r="Q160" t="inlineStr">
         <is>
-          <t>21/12/2023 17:59</t>
+          <t>21/12/2023 17:55</t>
         </is>
       </c>
       <c r="R160" t="n">
-        <v>3.82</v>
+        <v>7</v>
       </c>
       <c r="S160" t="inlineStr">
         <is>
-          <t>14/12/2023 18:13</t>
+          <t>14/12/2023 18:12</t>
         </is>
       </c>
       <c r="T160" t="n">
-        <v>3.36</v>
+        <v>5.26</v>
       </c>
       <c r="U160" t="inlineStr">
         <is>
-          <t>21/12/2023 17:59</t>
+          <t>21/12/2023 17:57</t>
         </is>
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/turkey/super-lig/ankaragucu-hatayspor/Iw6iNEIm/</t>
+          <t>https://www.betexplorer.com/football/turkey/super-lig/besiktas-alanyaspor/l41mOf3s/</t>
         </is>
       </c>
     </row>
@@ -15753,71 +15753,71 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Kasimpasa</t>
+          <t>Alanyaspor</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Rizespor</t>
+          <t>Samsunspor</t>
         </is>
       </c>
       <c r="I167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J167" t="n">
-        <v>1.93</v>
+        <v>2.59</v>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>21/12/2023 15:12</t>
+          <t>21/12/2023 18:12</t>
         </is>
       </c>
       <c r="L167" t="n">
-        <v>2.45</v>
+        <v>2.74</v>
       </c>
       <c r="M167" t="inlineStr">
         <is>
-          <t>25/12/2023 14:58</t>
+          <t>25/12/2023 14:53</t>
         </is>
       </c>
       <c r="N167" t="n">
-        <v>3.8</v>
+        <v>3.46</v>
       </c>
       <c r="O167" t="inlineStr">
         <is>
-          <t>21/12/2023 15:12</t>
+          <t>21/12/2023 18:12</t>
         </is>
       </c>
       <c r="P167" t="n">
-        <v>3.68</v>
+        <v>3.24</v>
       </c>
       <c r="Q167" t="inlineStr">
         <is>
-          <t>25/12/2023 14:58</t>
+          <t>25/12/2023 14:55</t>
         </is>
       </c>
       <c r="R167" t="n">
-        <v>3.87</v>
+        <v>2.76</v>
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>21/12/2023 15:12</t>
+          <t>21/12/2023 18:12</t>
         </is>
       </c>
       <c r="T167" t="n">
-        <v>2.87</v>
+        <v>2.83</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
-          <t>25/12/2023 14:58</t>
+          <t>25/12/2023 14:51</t>
         </is>
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/turkey/super-lig/kasimpasa-rizespor/nJc8JWHC/</t>
+          <t>https://www.betexplorer.com/football/turkey/super-lig/alanyaspor-samsunspor/Q9dCIjXI/</t>
         </is>
       </c>
     </row>
@@ -15845,71 +15845,71 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Alanyaspor</t>
+          <t>Kasimpasa</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Samsunspor</t>
+          <t>Rizespor</t>
         </is>
       </c>
       <c r="I168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J168" t="n">
-        <v>2.59</v>
+        <v>1.93</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>21/12/2023 18:12</t>
+          <t>21/12/2023 15:12</t>
         </is>
       </c>
       <c r="L168" t="n">
-        <v>2.74</v>
+        <v>2.45</v>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>25/12/2023 14:53</t>
+          <t>25/12/2023 14:58</t>
         </is>
       </c>
       <c r="N168" t="n">
-        <v>3.46</v>
+        <v>3.8</v>
       </c>
       <c r="O168" t="inlineStr">
         <is>
-          <t>21/12/2023 18:12</t>
+          <t>21/12/2023 15:12</t>
         </is>
       </c>
       <c r="P168" t="n">
-        <v>3.24</v>
+        <v>3.68</v>
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>25/12/2023 14:55</t>
+          <t>25/12/2023 14:58</t>
         </is>
       </c>
       <c r="R168" t="n">
-        <v>2.76</v>
+        <v>3.87</v>
       </c>
       <c r="S168" t="inlineStr">
         <is>
-          <t>21/12/2023 18:12</t>
+          <t>21/12/2023 15:12</t>
         </is>
       </c>
       <c r="T168" t="n">
-        <v>2.83</v>
+        <v>2.87</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
-          <t>25/12/2023 14:51</t>
+          <t>25/12/2023 14:58</t>
         </is>
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/turkey/super-lig/alanyaspor-samsunspor/Q9dCIjXI/</t>
+          <t>https://www.betexplorer.com/football/turkey/super-lig/kasimpasa-rizespor/nJc8JWHC/</t>
         </is>
       </c>
     </row>
@@ -16094,6 +16094,98 @@
       <c r="V170" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/turkey/super-lig/pendikspor-ankaragucu/hdb4KC26/</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>turkey</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>super-lig</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E171" s="2" t="n">
+        <v>45296.625</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Gaziantep</t>
+        </is>
+      </c>
+      <c r="G171" t="n">
+        <v>2</v>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Pendikspor</t>
+        </is>
+      </c>
+      <c r="I171" t="n">
+        <v>2</v>
+      </c>
+      <c r="J171" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>28/12/2024 15:42</t>
+        </is>
+      </c>
+      <c r="L171" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:56</t>
+        </is>
+      </c>
+      <c r="N171" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>28/12/2024 15:42</t>
+        </is>
+      </c>
+      <c r="P171" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:56</t>
+        </is>
+      </c>
+      <c r="R171" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>28/12/2024 15:42</t>
+        </is>
+      </c>
+      <c r="T171" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="U171" t="inlineStr">
+        <is>
+          <t>05/01/2024 14:56</t>
+        </is>
+      </c>
+      <c r="V171" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/turkey/super-lig/gaziantep-pendikspor/bTuUgDgP/</t>
         </is>
       </c>
     </row>

</xml_diff>